<commit_message>
feat(auth): created the controller, validator and routes for the authentification.
</commit_message>
<xml_diff>
--- a/doc/routes-needed.xlsx
+++ b/doc/routes-needed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ps46bhd\Desktop\Flashcards-P_Bulle\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DEEAC5-6B10-4A2F-AE98-4EDE8C73837F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E8B116F-4B7E-4535-B6FC-92110F5CB21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,21 +74,12 @@
     <t>register</t>
   </si>
   <si>
-    <t>/register</t>
-  </si>
-  <si>
     <t>login</t>
   </si>
   <si>
-    <t>/login</t>
-  </si>
-  <si>
     <t>logout</t>
   </si>
   <si>
-    <t>/logout</t>
-  </si>
-  <si>
     <t>JSON</t>
   </si>
   <si>
@@ -195,6 +186,15 @@
   </si>
   <si>
     <t>permet également de publier le deck</t>
+  </si>
+  <si>
+    <t>/users/login</t>
+  </si>
+  <si>
+    <t>/users/logout</t>
+  </si>
+  <si>
+    <t>/users/register</t>
   </si>
 </sst>
 </file>
@@ -564,7 +564,7 @@
   <dimension ref="A2:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +582,7 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -597,10 +597,10 @@
         <v>7</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -608,40 +608,40 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="H4" s="6"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>2</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="F5" s="7" t="s">
         <v>8</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>11</v>
@@ -660,68 +660,68 @@
         <v>2</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>12</v>
+        <v>52</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>8</v>
@@ -731,101 +731,101 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>8</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H14" s="6"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G15" s="6"/>
       <c r="H15" s="6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
@@ -841,41 +841,41 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>1</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
@@ -887,22 +887,22 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H20" s="6"/>
       <c r="O20" s="1"/>
@@ -913,22 +913,22 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="H21" s="6"/>
       <c r="O21" s="1"/>
@@ -939,19 +939,19 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>4</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>

</xml_diff>